<commit_message>
restauranteLong/Lat -> DECIMAL(6,3) (ajustado para ser igual aodbSblenders.sql)
</commit_message>
<xml_diff>
--- a/PastaDDSblenders.xlsx
+++ b/PastaDDSblenders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Computery\Desktop\bancoTCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEA73D4-B602-41FF-AE94-598E0A94689F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49719AF-3A0C-4645-A93C-763932F86961}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-120" windowWidth="23280" windowHeight="13740" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="-120" windowWidth="23190" windowHeight="13740" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TipoAgente" sheetId="13" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="163">
   <si>
     <t>Tipo de Dado</t>
   </si>
@@ -97,9 +97,6 @@
     <t>longRestaurante</t>
   </si>
   <si>
-    <t>XXX,XX</t>
-  </si>
-  <si>
     <t>Longitude do Restaurante</t>
   </si>
   <si>
@@ -533,6 +530,12 @@
   </si>
   <si>
     <t>Identificador do agente do totem</t>
+  </si>
+  <si>
+    <t>6, 3</t>
+  </si>
+  <si>
+    <t>XXX,XXX</t>
   </si>
 </sst>
 </file>
@@ -899,6 +902,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -926,7 +930,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2214,44 +2217,44 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2303,87 +2306,87 @@
         <v>4</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F2" s="6">
         <v>32</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F3" s="6">
         <v>32</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F4" s="6">
         <v>32</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F5" s="6">
         <v>5</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2434,15 +2437,15 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -2450,21 +2453,21 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>9</v>
@@ -2474,14 +2477,14 @@
         <v>15</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2494,10 +2497,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2531,12 +2534,12 @@
         <v>4</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -2554,12 +2557,12 @@
         <v>1</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>9</v>
@@ -2586,10 +2589,10 @@
         <v>13</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="6">
-        <v>5.2</v>
+        <v>162</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>161</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>14</v>
@@ -2607,23 +2610,30 @@
         <v>13</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="6">
-        <v>5.2</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="F5" s="6">
         <v>240</v>
       </c>
       <c r="G5" s="6"/>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="27"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2667,15 +2677,15 @@
         <v>4</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -2687,21 +2697,21 @@
         <v>7</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>6</v>
@@ -2713,21 +2723,21 @@
         <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="6">
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>6</v>
@@ -2739,7 +2749,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="6">
         <v>20</v>
@@ -2796,15 +2806,15 @@
         <v>4</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -2816,21 +2826,21 @@
         <v>7</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>6</v>
@@ -2842,21 +2852,21 @@
         <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="6">
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>9</v>
@@ -2868,30 +2878,30 @@
         <v>50</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="H4" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="6">
         <v>5.2</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="6">
         <v>2</v>
@@ -2899,7 +2909,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>9</v>
@@ -2911,101 +2921,101 @@
         <v>200</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="27" t="s">
+      <c r="A7" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3065,15 +3075,15 @@
         <v>4</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -3085,21 +3095,21 @@
         <v>7</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>9</v>
@@ -3111,14 +3121,14 @@
         <v>30</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3170,15 +3180,15 @@
         <v>4</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -3190,21 +3200,21 @@
         <v>7</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>6</v>
@@ -3216,21 +3226,21 @@
         <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3" s="6">
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>9</v>
@@ -3242,131 +3252,131 @@
         <v>50</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="H4" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="6">
         <v>5.2</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" s="6">
         <v>20.55</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" s="30" t="s">
+      <c r="A6" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
+      <c r="E6" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="34"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>9</v>
@@ -3378,10 +3388,10 @@
         <v>300</v>
       </c>
       <c r="E14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -3449,15 +3459,15 @@
         <v>4</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -3469,21 +3479,21 @@
         <v>7</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>9</v>
@@ -3495,13 +3505,13 @@
         <v>30</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="H3" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3559,52 +3569,52 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -3613,53 +3623,53 @@
         <v>254</v>
       </c>
       <c r="E4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" t="s">
         <v>153</v>
       </c>
-      <c r="F4" t="s">
-        <v>154</v>
-      </c>
       <c r="H4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5">
         <v>64</v>
       </c>
       <c r="E5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F5" t="s">
         <v>156</v>
       </c>
-      <c r="F5" t="s">
-        <v>157</v>
-      </c>
       <c r="H5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D6">
         <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -3714,95 +3724,95 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -3811,18 +3821,18 @@
         <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -3831,27 +3841,27 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -3904,35 +3914,35 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -3941,13 +3951,13 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" t="s">
         <v>124</v>
       </c>
-      <c r="F3" t="s">
-        <v>125</v>
-      </c>
       <c r="H3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3962,7 +3972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{868612A4-0641-41F0-8554-702C4BA3595D}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -3998,74 +4008,74 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D16" s="36"/>
+      <c r="D16" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -4115,15 +4125,15 @@
         <v>4</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>6</v>
@@ -4131,21 +4141,21 @@
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2" s="25">
         <v>1</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>6</v>
@@ -4153,21 +4163,21 @@
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
       <c r="E3" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F3" s="25">
         <v>1</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>9</v>
@@ -4177,19 +4187,19 @@
         <v>50</v>
       </c>
       <c r="E4" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" s="25" t="s">
         <v>141</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>142</v>
       </c>
       <c r="G4" s="16"/>
       <c r="H4" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>9</v>
@@ -4199,54 +4209,54 @@
         <v>50</v>
       </c>
       <c r="E5" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="25" t="s">
         <v>144</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>145</v>
       </c>
       <c r="G5" s="16"/>
       <c r="H5" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="16">
         <v>32</v>
       </c>
       <c r="E6" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" s="25" t="s">
         <v>147</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>148</v>
       </c>
       <c r="G6" s="16"/>
       <c r="H6" s="17"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>149</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>150</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F7" s="25">
         <v>0</v>
       </c>
       <c r="G7" s="16"/>
       <c r="H7" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4321,104 +4331,104 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2">
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3">
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" t="s">
         <v>57</v>
-      </c>
-      <c r="E4" t="s">
-        <v>58</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5">
         <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F6" s="2">
         <v>38431</v>
@@ -4426,7 +4436,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -4435,10 +4445,10 @@
         <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.25">
@@ -4493,84 +4503,84 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2">
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3">
         <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4">
         <v>245</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4624,15 +4634,15 @@
         <v>4</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>6</v>
@@ -4640,21 +4650,21 @@
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F2" s="13">
         <v>12</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>6</v>
@@ -4662,21 +4672,21 @@
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" s="13">
         <v>34</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>6</v>
@@ -4684,41 +4694,41 @@
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4" s="13">
         <v>5</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="13">
         <v>5</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>6</v>
@@ -4726,16 +4736,16 @@
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
       <c r="E6" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F6" s="15">
         <v>54</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionado atributo instrucoes para a tabela pedido
</commit_message>
<xml_diff>
--- a/PastaDDSblenders.xlsx
+++ b/PastaDDSblenders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Computery\Desktop\bancoTCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49719AF-3A0C-4645-A93C-763932F86961}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20EEAF0-38C8-4AAF-8408-73F8B807A323}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="-120" windowWidth="23190" windowHeight="13740" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="-120" windowWidth="23190" windowHeight="13740" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TipoAgente" sheetId="13" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="166">
   <si>
     <t>Tipo de Dado</t>
   </si>
@@ -536,6 +536,15 @@
   </si>
   <si>
     <t>XXX,XXX</t>
+  </si>
+  <si>
+    <t>instrucoes</t>
+  </si>
+  <si>
+    <t>Instruções especiais para o pedido</t>
+  </si>
+  <si>
+    <t>Remover tomates-cereja da salada</t>
   </si>
 </sst>
 </file>
@@ -1849,8 +1858,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BA6443AC-FE50-4A17-B098-01A2C3A32388}" name="Tabela7" displayName="Tabela7" ref="A1:H7" totalsRowShown="0">
-  <autoFilter ref="A1:H7" xr:uid="{4A595268-F932-43C3-B17D-EB5B187F831B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BA6443AC-FE50-4A17-B098-01A2C3A32388}" name="Tabela7" displayName="Tabela7" ref="A1:H8" totalsRowShown="0">
+  <autoFilter ref="A1:H8" xr:uid="{4A595268-F932-43C3-B17D-EB5B187F831B}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0C675AF5-86B1-489D-9712-2CFAB9F64066}" name="Nome do Campo"/>
     <tableColumn id="2" xr3:uid="{DC4207C1-F9CC-4332-9942-E67DD90516F3}" name="Tipo de Dado"/>
@@ -2499,7 +2508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -4295,8 +4304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276B064F-029E-484B-87E7-F731F31E8A56}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4449,6 +4458,23 @@
       </c>
       <c r="F7" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>280</v>
+      </c>
+      <c r="E8" t="s">
+        <v>164</v>
+      </c>
+      <c r="F8" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>